<commit_message>
redesign, logo and audio connector changed
</commit_message>
<xml_diff>
--- a/PCB/bom.xlsx
+++ b/PCB/bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="107">
   <si>
     <t>Id</t>
   </si>
@@ -94,15 +94,6 @@
     <t>Jumper_NC_Small</t>
   </si>
   <si>
-    <t>P104</t>
-  </si>
-  <si>
-    <t>LUM150302</t>
-  </si>
-  <si>
-    <t>Audio Out</t>
-  </si>
-  <si>
     <t>R102</t>
   </si>
   <si>
@@ -250,9 +241,6 @@
     <t>ERJ-3GEY0R00V</t>
   </si>
   <si>
-    <t>Lumberg 1503 02</t>
-  </si>
-  <si>
     <t>ERJ3EKF2700V</t>
   </si>
   <si>
@@ -328,10 +316,25 @@
     <t>PJ-102B</t>
   </si>
   <si>
-    <t>Reichelt</t>
-  </si>
-  <si>
     <t>147873-1</t>
+  </si>
+  <si>
+    <t>Thonk</t>
+  </si>
+  <si>
+    <t>J101</t>
+  </si>
+  <si>
+    <t>Thonkicon</t>
+  </si>
+  <si>
+    <t>AUOUT</t>
+  </si>
+  <si>
+    <t>PJ301M-12</t>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/3-5mm-jacks/</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1216,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:I30"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,7 +1229,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1244,15 +1247,15 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1270,19 +1273,19 @@
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B3">
         <f>B2+1</f>
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1294,12 +1297,12 @@
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B28" si="0">B3+1</f>
@@ -1318,12 +1321,12 @@
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
@@ -1342,12 +1345,12 @@
         <v>13</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
@@ -1366,12 +1369,12 @@
         <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
@@ -1390,12 +1393,12 @@
         <v>19</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
@@ -1414,12 +1417,12 @@
         <v>22</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -1438,43 +1441,46 @@
         <v>25</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="G10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="I10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
@@ -1486,19 +1492,19 @@
         <v>270</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
         <v>24</v>
@@ -1510,19 +1516,19 @@
         <v>680</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
         <v>24</v>
@@ -1534,19 +1540,19 @@
         <v>330</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>24</v>
@@ -1555,172 +1561,172 @@
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E15">
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1729,145 +1735,145 @@
         <v>4050</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="16.899999999999999" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E22">
         <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E24">
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E25">
         <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G26" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -1876,34 +1882,34 @@
         <v>25</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E28">
         <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1911,7 +1917,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G30" s="4"/>
     </row>
@@ -1937,6 +1943,6 @@
     <hyperlink ref="G6" r:id="rId18" display="http://www.mouser.de/ProductDetail/CUI/PJ-102B/?qs=sGAEpiMZZMtnOp%252bbbqA009lE0K0K%252bPZGwBn8mNs%2f67swvqoafgHXxg%3d%3d"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>